<commit_message>
fix some instruction type error
</commit_message>
<xml_diff>
--- a/docs/excels/RV32_instructions.xlsx
+++ b/docs/excels/RV32_instructions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="16305" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="RV32I" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="164">
   <si>
     <t>分类</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -202,12 +208,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -276,12 +276,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -439,12 +433,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -513,12 +501,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -587,12 +569,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -657,16 +633,78 @@
     <t>XORI</t>
   </si>
   <si>
+    <t>Exclusive-OR Immediate</t>
+  </si>
+  <si>
+    <r>
+      <t>x[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
+      <t>rd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
+      <t>] = x[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.25"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
+      <t>rs1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
+      <t>] ^ sext[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA635E1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
+      <t>imm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>xori rd, rs, imm</t>
+  </si>
+  <si>
+    <t>ORI</t>
+  </si>
+  <si>
     <t>OR Immediate</t>
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -703,7 +741,7 @@
         <rFont val="仿宋"/>
         <charset val="134"/>
       </rPr>
-      <t>] ^ sext[</t>
+      <t>] | sext[</t>
     </r>
     <r>
       <rPr>
@@ -725,9 +763,6 @@
     </r>
   </si>
   <si>
-    <t>xori rd, rs, imm</t>
-  </si>
-  <si>
     <t>ANDI</t>
   </si>
   <si>
@@ -735,12 +770,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -812,12 +841,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -874,12 +897,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>M[ x[</t>
     </r>
     <r>
@@ -948,12 +965,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>M[ x[</t>
     </r>
     <r>
@@ -1022,12 +1033,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>M[ x[</t>
     </r>
     <r>
@@ -1102,12 +1107,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1176,12 +1175,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1250,12 +1243,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1324,12 +1311,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1398,12 +1379,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1472,12 +1447,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1546,12 +1515,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1620,12 +1583,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1691,12 +1648,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1765,12 +1716,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1839,12 +1784,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1901,12 +1840,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>if (x[</t>
     </r>
     <r>
@@ -1975,12 +1908,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>if ( x[</t>
     </r>
     <r>
@@ -2049,12 +1976,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>if ( (signed) x[</t>
     </r>
     <r>
@@ -2123,12 +2044,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>if ( (signed) x[</t>
     </r>
     <r>
@@ -2197,12 +2112,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>if ( x[</t>
     </r>
     <r>
@@ -2271,12 +2180,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>if ( x[</t>
     </r>
     <r>
@@ -2345,12 +2248,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -2423,12 +2320,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="仿宋"/>
-        <charset val="134"/>
-      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -2519,10 +2410,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="仿宋"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3281,7 +3174,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3300,28 +3193,34 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3854,10 +3753,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -4073,224 +3972,222 @@
       <c r="E12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>52</v>
-      </c>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="F13" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="E14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="C15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="E15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="F15" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="E17" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="F17" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="5"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="C18" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="E18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="5"/>
-      <c r="B19" s="8"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>
-      <c r="B20" s="8"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="E20" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="6" t="s">
+      <c r="F20" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="5"/>
-      <c r="B21" s="8"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="F21" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="5"/>
-      <c r="B22" s="8"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="5"/>
-      <c r="B23" s="8"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="E23" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="F23" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="5"/>
-      <c r="B24" s="8"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="5"/>
-      <c r="B25" s="8"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="11" t="s">
         <v>107</v>
       </c>
       <c r="F25" s="9" t="s">
@@ -4299,230 +4196,246 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="5"/>
-      <c r="B26" s="8"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>109</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="F26" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="F27" s="9" t="s">
         <v>115</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="E28" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="F28" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="C29" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E29" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="F29" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="F30" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="E31" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="F31" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="F32" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="F33" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="9" t="s">
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="34" ht="27" spans="1:6">
-      <c r="A34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="6" t="s">
+      <c r="E34" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="F34" s="7" t="s">
         <v>145</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="35" ht="27" spans="1:6">
       <c r="A35" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="E35" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D35" s="8" t="s">
+      <c r="F35" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E35" s="11" t="s">
+    </row>
+    <row r="36" ht="27" spans="1:6">
+      <c r="A36" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="B36" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="5" t="s">
+      <c r="C36" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="6" t="s">
+      <c r="E36" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="F36" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="12" t="s">
+      <c r="A37" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="E37" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="F37" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="F37" s="13" t="s">
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="5"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="14" t="s">
         <v>160</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A27"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B26"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B27"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="B37:B38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add M extension instruction to excel table
</commit_message>
<xml_diff>
--- a/docs/excels/RV32_instructions.xlsx
+++ b/docs/excels/RV32_instructions.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16305" windowHeight="7800"/>
+    <workbookView windowWidth="24045" windowHeight="12375" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RV32I" sheetId="1" r:id="rId1"/>
+    <sheet name="RV32M" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="198">
   <si>
     <t>分类</t>
   </si>
@@ -208,6 +209,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -276,6 +284,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -433,6 +448,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -501,6 +523,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -569,6 +598,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -637,6 +673,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -705,6 +748,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -770,6 +820,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -841,6 +898,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -897,6 +960,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>M[ x[</t>
     </r>
     <r>
@@ -965,6 +1034,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>M[ x[</t>
     </r>
     <r>
@@ -1033,6 +1108,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>M[ x[</t>
     </r>
     <r>
@@ -1107,6 +1188,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1175,6 +1262,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1243,6 +1336,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1311,6 +1410,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1379,6 +1484,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1447,6 +1558,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1515,6 +1632,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1583,6 +1706,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1648,6 +1777,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1716,6 +1851,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1784,6 +1925,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -1840,6 +1987,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>if (x[</t>
     </r>
     <r>
@@ -1908,6 +2061,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>if ( x[</t>
     </r>
     <r>
@@ -1976,6 +2135,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>if ( (signed) x[</t>
     </r>
     <r>
@@ -2044,6 +2209,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>if ( (signed) x[</t>
     </r>
     <r>
@@ -2112,6 +2283,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>if ( x[</t>
     </r>
     <r>
@@ -2180,6 +2357,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>if ( x[</t>
     </r>
     <r>
@@ -2248,6 +2431,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -2320,6 +2509,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="仿宋"/>
+        <charset val="134"/>
+      </rPr>
       <t>x[</t>
     </r>
     <r>
@@ -2389,6 +2584,108 @@
   </si>
   <si>
     <t>ebreak</t>
+  </si>
+  <si>
+    <t>Mul</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>x[rd] = (u32) x[rs1] * (u32) x[rs2]</t>
+  </si>
+  <si>
+    <t>mul rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>MULH</t>
+  </si>
+  <si>
+    <t>Multiply high</t>
+  </si>
+  <si>
+    <t>x[rd] = ((s64) x[rs1] * (s64) x[rs2]) &gt;&gt; XLEN</t>
+  </si>
+  <si>
+    <t>mulh rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>MULHSU</t>
+  </si>
+  <si>
+    <t>Multiply high, signed-unsigned</t>
+  </si>
+  <si>
+    <t>x[rd] = ((s64) x[rs1] * (u64) x[rs2]) &gt;&gt; XLEN</t>
+  </si>
+  <si>
+    <t>mulhsu rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>MULHU</t>
+  </si>
+  <si>
+    <t>Multiply high, unsigned</t>
+  </si>
+  <si>
+    <t>x[rd] = ((u64) x[rs1] * (u64) x[rs2]) &gt;&gt; XLEN</t>
+  </si>
+  <si>
+    <t>mulhu rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>Divide</t>
+  </si>
+  <si>
+    <t>x[rd] = (s32) x[rs1] / (s32) x[rs2]</t>
+  </si>
+  <si>
+    <t>div rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>DIVU</t>
+  </si>
+  <si>
+    <t>Divide, unsigned</t>
+  </si>
+  <si>
+    <t>x[rd] = (u32) x[rs1] / (u32) x[rs2]</t>
+  </si>
+  <si>
+    <t>divu rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>REM</t>
+  </si>
+  <si>
+    <t>Remainder</t>
+  </si>
+  <si>
+    <t>x[rd] = (s32) x[rs1] % (s32) x[rs2]</t>
+  </si>
+  <si>
+    <t>rem rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t>REMU</t>
+  </si>
+  <si>
+    <t>Remainder, unsigned</t>
+  </si>
+  <si>
+    <t>x[rd] = (u32) x[rs1] % (u32) x[rs2]</t>
+  </si>
+  <si>
+    <t>remu, rd, rs1, rs2</t>
   </si>
 </sst>
 </file>
@@ -3174,13 +3471,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3197,6 +3491,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3755,670 +4076,670 @@
   <sheetPr/>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="8.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46" style="1" customWidth="1"/>
-    <col min="5" max="5" width="67.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="10.375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="9" style="15"/>
+    <col min="3" max="3" width="8.875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="46" style="15" customWidth="1"/>
+    <col min="5" max="5" width="67.125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="34.875" style="15" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="9"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="17" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="8" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="17" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="5"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="6" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="8" t="s">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="8" t="s">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="17" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="8" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6" t="s">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="8" t="s">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="17" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6" t="s">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="8" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="17" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="17" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="5"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="6" t="s">
+      <c r="A30" s="4"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="5"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8" t="s">
+      <c r="A31" s="4"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F31" s="17" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="5"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="6" t="s">
+      <c r="A32" s="4"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="5"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8" t="s">
+      <c r="A33" s="4"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="17" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="5"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="6" t="s">
+      <c r="A34" s="4"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="35" ht="27" spans="1:6">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="17" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="36" ht="27" spans="1:6">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="E37" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="17" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="5"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="14" t="s">
+      <c r="A38" s="4"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="22" t="s">
         <v>162</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="23" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4440,4 +4761,185 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="4" max="4" width="32.625" customWidth="1"/>
+    <col min="5" max="5" width="53.5" customWidth="1"/>
+    <col min="6" max="6" width="22.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B2:B9"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>